<commit_message>
Updated pipeToExcel to include piping accessories and show family names in additional column.
</commit_message>
<xml_diff>
--- a/PipeMiniSchedule.xlsx
+++ b/PipeMiniSchedule.xlsx
@@ -1,49 +1,81 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RIchardC\Documents\Personal Projects\Dynamo Scripts\PipeCalculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34289419-36C4-4003-A782-18F921AEF142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E7A383-BA8A-4DAB-82EB-43303B3DFEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41955" yWindow="4050" windowWidth="18900" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CHWS" sheetId="2" r:id="rId1"/>
-    <sheet name="CHWR" sheetId="3" r:id="rId2"/>
-    <sheet name="HWS" sheetId="4" r:id="rId3"/>
-    <sheet name="HWR" sheetId="5" r:id="rId4"/>
+    <sheet name="CHW B" sheetId="10" r:id="rId1"/>
+    <sheet name="HW B" sheetId="15" r:id="rId2"/>
+    <sheet name="BASEMENT B CHW" sheetId="7" state="hidden" r:id="rId3"/>
+    <sheet name="LEVEL 1 B CHW" sheetId="19" state="hidden" r:id="rId4"/>
+    <sheet name="RISER B CHW" sheetId="18" state="hidden" r:id="rId5"/>
+    <sheet name="LEVEL 6 B CHW" sheetId="17" state="hidden" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="7">
   <si>
-    <t>3/4 in</t>
+    <t>3 in</t>
   </si>
   <si>
-    <t>1/2 in</t>
+    <t>4 in</t>
+  </si>
+  <si>
+    <t>2 in</t>
+  </si>
+  <si>
+    <t>BASEMENT</t>
+  </si>
+  <si>
+    <t>LEVEL 1</t>
+  </si>
+  <si>
+    <t>RISER</t>
+  </si>
+  <si>
+    <t>LEVEL 6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -69,9 +101,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,165 +386,680 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F9AD5AB-63CE-46BF-9A9C-8BEF41118264}">
-  <dimension ref="E5:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{277BE4C0-16E5-4C62-954A-2F3A561B18BC}">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="5" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E6" s="1"/>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3">
+        <v>5.1041666666666297</v>
+      </c>
+      <c r="D1" s="3">
+        <v>32.549999999999997</v>
+      </c>
+      <c r="E1">
+        <v>2.33</v>
+      </c>
+      <c r="F1">
+        <f>C1*E1/100</f>
+        <v>0.11892708333333248</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3">
+        <v>8.3481873082918305</v>
+      </c>
+      <c r="D2" s="3">
+        <v>32.549999999999997</v>
+      </c>
+      <c r="E2">
+        <v>2.33</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F21" si="0">C2*E2/100</f>
+        <v>0.19451276428319964</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1.9801645069417999</v>
+      </c>
+      <c r="D3" s="3">
+        <f>D2+2.43*3</f>
+        <v>39.839999999999996</v>
+      </c>
+      <c r="E3">
+        <v>3.35</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>6.6335510982550291E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2.4302553313947</v>
+      </c>
+      <c r="D4" s="3">
+        <v>39.840000000000003</v>
+      </c>
+      <c r="E4">
+        <v>3.35</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" si="0"/>
+        <v>8.1413553601722449E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.42057981442026798</v>
+      </c>
+      <c r="D5" s="3">
+        <v>39.840000000000003</v>
+      </c>
+      <c r="E5">
+        <v>3.35</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="0"/>
+        <v>1.4089423783078979E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3">
+        <v>56.6041666666666</v>
+      </c>
+      <c r="D6" s="3">
+        <v>39.840000000000003</v>
+      </c>
+      <c r="E6">
+        <v>3.35</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="0"/>
+        <v>1.8962395833333312</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1.14756605666981</v>
+      </c>
+      <c r="D7" s="3">
+        <v>39.840000000000003</v>
+      </c>
+      <c r="E7">
+        <v>3.35</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8443462898438641E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3">
+        <v>7.8306352165017801</v>
+      </c>
+      <c r="D8" s="3">
+        <v>39.840000000000003</v>
+      </c>
+      <c r="E8">
+        <v>3.35</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="0"/>
+        <v>0.26232627975280964</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3">
+        <v>21.9140201332985</v>
+      </c>
+      <c r="D9" s="3">
+        <v>39.840000000000003</v>
+      </c>
+      <c r="E9">
+        <v>3.35</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="0"/>
+        <v>0.73411967446549975</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3">
+        <v>24.396983416151301</v>
+      </c>
+      <c r="D10" s="3">
+        <v>39.840000000000003</v>
+      </c>
+      <c r="E10">
+        <v>3.35</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="0"/>
+        <v>0.81729894444106865</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3">
+        <v>5.31382527313965</v>
+      </c>
+      <c r="D11" s="3">
+        <v>39.840000000000003</v>
+      </c>
+      <c r="E11">
+        <v>3.35</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="0"/>
+        <v>0.17801314665017828</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3">
+        <v>13.2678616806779</v>
+      </c>
+      <c r="D12" s="3">
+        <v>39.840000000000003</v>
+      </c>
+      <c r="E12">
+        <v>3.35</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="0"/>
+        <v>0.44447336630270967</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3">
+        <v>5.8375847259481501</v>
+      </c>
+      <c r="D13" s="3">
+        <v>39.840000000000003</v>
+      </c>
+      <c r="E13">
+        <v>3.35</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="0"/>
+        <v>0.19555908831926302</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3">
+        <v>5.9315304161026399</v>
+      </c>
+      <c r="D14" s="3">
+        <v>39.840000000000003</v>
+      </c>
+      <c r="E14">
+        <v>3.35</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="0"/>
+        <v>0.19870626893943844</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3">
+        <v>13.348281250000101</v>
+      </c>
+      <c r="D15" s="3">
+        <f>D14+189.95+53+1.53+5.5</f>
+        <v>289.81999999999994</v>
+      </c>
+      <c r="E15">
+        <v>4.57</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="0"/>
+        <v>0.61001645312500463</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.66541538623058305</v>
+      </c>
+      <c r="D16" s="3">
+        <v>289.82</v>
+      </c>
+      <c r="E16">
+        <v>4.57</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="0"/>
+        <v>3.0409483150737646E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3">
+        <v>5.4021169430128397</v>
+      </c>
+      <c r="D17" s="3">
+        <f>D16+10.6</f>
+        <v>300.42</v>
+      </c>
+      <c r="E17">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="0"/>
+        <v>0.26416351851332787</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.64914062510191295</v>
+      </c>
+      <c r="D18" s="3">
+        <v>300.42</v>
+      </c>
+      <c r="E18">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="F18" s="3">
+        <f t="shared" si="0"/>
+        <v>3.1742976567483538E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3">
+        <v>12.4887972302413</v>
+      </c>
+      <c r="D19" s="3">
+        <v>300.42</v>
+      </c>
+      <c r="E19">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.61070218455879954</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3">
+        <v>3.5155924955326299</v>
+      </c>
+      <c r="D20" s="3">
+        <v>300.42</v>
+      </c>
+      <c r="E20">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="F20" s="3">
+        <f t="shared" si="0"/>
+        <v>0.17191247303154558</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3">
+        <v>3.5155924955326299</v>
+      </c>
+      <c r="D21" s="3">
+        <v>300.42</v>
+      </c>
+      <c r="E21">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" si="0"/>
+        <v>0.17191247303154558</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <f>SUM(C1:C21)</f>
+        <v>200.11246363852359</v>
+      </c>
+      <c r="F22">
+        <f>SUM(F1:F21)</f>
+        <v>7.1313177130650649</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <f>C22*2</f>
+        <v>400.22492727704719</v>
+      </c>
+      <c r="F23">
+        <f>F22*2</f>
+        <v>14.26263542613013</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F24" s="1">
+        <f>F23+14</f>
+        <v>28.262635426130132</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F25" s="1">
+        <f>F24*1.25</f>
+        <v>35.328294282662668</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F28" s="1"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G30" s="4"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F476AF4E-C3BE-4C77-8335-9686C73773CE}">
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="B1:G29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G29" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59AC9D6F-1D4A-4165-9F64-40BD48A11F82}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07FC381C-2D90-4398-8B88-25E33027C0A6}">
+  <sheetPr codeName="Sheet10"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79429FB7-3F19-490D-837B-65F26B1CFF95}">
-  <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1">
-        <v>13.911623543971</v>
+        <v>0.66541538623058305</v>
       </c>
       <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>8.18</v>
-      </c>
-      <c r="E1">
-        <v>40.9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>1.27767983978363</v>
+        <v>5.4021169430128397</v>
       </c>
       <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>40.94</v>
-      </c>
-      <c r="E2">
-        <v>204.7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1.7843373216041201</v>
+        <v>0.64914062510191295</v>
       </c>
       <c r="C3">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>56.58</v>
-      </c>
-      <c r="E3">
-        <v>282.89999999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4">
-        <v>2.48133580782262</v>
+        <v>12.4887972302413</v>
       </c>
       <c r="C4">
-        <v>8</v>
-      </c>
-      <c r="D4">
-        <v>94.48</v>
-      </c>
-      <c r="E4">
-        <v>472.4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5">
-        <v>3.8738870632556601</v>
+        <v>3.5155924955326299</v>
       </c>
       <c r="C5">
-        <v>9</v>
-      </c>
-      <c r="D5">
-        <v>116.63</v>
-      </c>
-      <c r="E5">
-        <v>583.15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6">
-        <v>2.0530688824596099</v>
+        <v>3.5155924955326299</v>
       </c>
       <c r="C6">
-        <v>12</v>
-      </c>
-      <c r="D6">
-        <v>195.46</v>
-      </c>
-      <c r="E6">
-        <v>977.3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>11.1770834962932</v>
-      </c>
-      <c r="C7">
-        <v>29</v>
-      </c>
-      <c r="D7">
-        <v>8.18</v>
-      </c>
-      <c r="E7">
-        <v>40.9</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -518,15 +1068,211 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC9A6F4-8ACB-4958-8A6F-6DDC2516FCCE}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1788928B-D2F4-4561-B58C-891F1ADC50CD}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1.14756605666981</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>7.8306352165017801</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>21.9140201332985</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>24.396983416151301</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>5.31382527313965</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>13.2678616806779</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>5.8375847259481501</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>5.9315304161026399</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>13.348281250000101</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85467CFE-0FD8-459E-8ED3-B589B75003FC}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>56.6041666666666</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B766C065-8D4C-4B8D-BBD7-1C1623EAC229}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>5.1041666666666297</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>8.3481873082918305</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1.9801645069417999</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>2.4302553313947</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0.42057981442026798</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>